<commit_message>
CSI1101 A2: v2 condensed version, needs bib then done
</commit_message>
<xml_diff>
--- a/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib_v2.xlsx
+++ b/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib_v2.xlsx
@@ -451,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:B6"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,27 +463,27 @@
     <col min="2" max="2" width="150.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CSI1101 A2: finished v2
</commit_message>
<xml_diff>
--- a/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib_v2.xlsx
+++ b/year_1/sem_2/CSI1101_computer_security/0b_assignment_2_[22MAY15_0900]/dev/bib_v2.xlsx
@@ -14,57 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Microsoft, 2008</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Microsoft. (2015). </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Microsoft Support Lifecycle</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Microsoft</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Retrieved February 27, 2015, from http://support.microsoft.com/lifecycle/search/default.aspx?alpha=Vista</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Baker, Hylender, &amp; Valentine, 2008, p. 2</t>
   </si>
@@ -75,46 +25,81 @@
     <t>O'Connor, 2008</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">O’Connor, E. (2008). </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BigAdmin Feature Article: Patch Management Best Practices</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. Retrieved May 13, 2015, from http://www.oracle.com/technetwork/systems/articles/patch-management-jsp-135385.html</t>
-    </r>
+    <t>Scarfone &amp; Souppaya, 2013</t>
+  </si>
+  <si>
+    <t>Tice, 2012</t>
+  </si>
+  <si>
+    <t>Microsoft, 2012</t>
+  </si>
+  <si>
+    <t>Oliver &amp; Snowden, 2015</t>
+  </si>
+  <si>
+    <t>Tice, K. [solarwindsinc]. (2012, September 12)  Patch Manager Guided Tour. Retrieved May 14, 2015, from https://www.youtube.com/watch?v=-DldViUL1d0</t>
+  </si>
+  <si>
+    <t>O’Connor, E. (2008). BigAdmin Feature Article: Patch Management Best Practices. Retrieved May 13, 2015, from http://www.oracle.com/technetwork/systems/articles/patch-management-jsp-135385.html</t>
+  </si>
+  <si>
+    <t>Scarfone, K., &amp; Souppaya, M. (2013). Guide to Enterprise Patch Management Technologies NIST Special Publication 800-40 Guide to Enterprise Patch Management Technologies. NIST. doi:10.6028/NIST.SP.800-40r3</t>
+  </si>
+  <si>
+    <t>Password must meet complexity requirements. (n.d.). Retrieved May 14, 2015, from https://technet.microsoft.com/en-us/library/hh994562(v=ws.10).aspx</t>
+  </si>
+  <si>
+    <t>Oliver, J., &amp; Snowden, E. [LastWeekTonight]. (2015, April 9). Last Week Tonight with John Oliver: Edward Snowden on Passwords. Retrieved May 6, 2015, from https://www.youtube.com/watch?v=yzGzB-yYKcc</t>
+  </si>
+  <si>
+    <t>Goodin, D. (2014). Stanford’s password policy shuns one-size-fits-all security | Ars Technica. Ars Technica. Retrieved April 30, 2015, from http://arstechnica.com/security/2014/04/25/stanfords-password-policy-shuns-one-size-fits-all-security/</t>
+  </si>
+  <si>
+    <t>Goodin, 2014</t>
+  </si>
+  <si>
+    <t>Machkovech, 2015</t>
+  </si>
+  <si>
+    <t>Machkovech, S. (2015). Hacked French network exposed its own passwords during TV interview | Ars Technica. Ars Technica. Retrieved May 6, 2015, from http://arstechnica.com/security/2015/04/09/hacked-french-network-exposed-its-own-passwords-during-tv-interview/</t>
+  </si>
+  <si>
+    <t>Microsoft, 2005a</t>
+  </si>
+  <si>
+    <t>Microsoft. (2005a). Apply or modify password policy: Logon and Authentication. Retrieved May 14, 2015, from https://technet.microsoft.com/en-au/library/cc781633(v=ws.10).aspx?f=255&amp;MSPPError=-2147217396#BKMK_3</t>
+  </si>
+  <si>
+    <t>Microsoft. (2005b). Assign user rights to a group in Active Directory: Active Directory. Retrieved May 14, 2015, from https://technet.microsoft.com/en-au/library/cc786658(v=ws.10).aspx</t>
+  </si>
+  <si>
+    <t>Microsoft, 2005b</t>
+  </si>
+  <si>
+    <t>Microsoft, n.d.-a</t>
+  </si>
+  <si>
+    <t>Microsoft. (n.d.-a). Screen Saver timeout. Retrieved May 14, 2015, from https://technet.microsoft.com/en-us/library/cc961876.aspx</t>
+  </si>
+  <si>
+    <t>Microsoft. (n.d.-b). What is User Account Control? - Windows Help. Retrieved March 14, 2015, from http://windows.microsoft.com/en-au/windows/what-is-user-account-control#1TC=windows-vista</t>
+  </si>
+  <si>
+    <t>Microsoft, n.d.-b</t>
+  </si>
+  <si>
+    <t>Microsoft. (2007). Configure UAC settings via policy - Microsoft Reduce Customer Effort Center - Site Home - TechNet Blogs. Retrieved May 14, 2015, from http://blogs.technet.com/b/asiasupp/archive/2007/02/08/configure-uac-settings-via-policy.aspx</t>
+  </si>
+  <si>
+    <t>Microsoft, 2007</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -142,10 +127,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,43 +440,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="150.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="150.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:B13">
+    <sortCondition ref="B5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>